<commit_message>
Frames per Second anpassbar
</commit_message>
<xml_diff>
--- a/Verkehrssimulation/doc/KW1442/Kurven.xlsx
+++ b/Verkehrssimulation/doc/KW1442/Kurven.xlsx
@@ -1060,11 +1060,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="392004040"/>
-        <c:axId val="392007736"/>
+        <c:axId val="2117731064"/>
+        <c:axId val="2117734760"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="392004040"/>
+        <c:axId val="2117731064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1106,7 +1106,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="392007736"/>
+        <c:crossAx val="2117734760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1114,7 +1114,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="392007736"/>
+        <c:axId val="2117734760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1165,7 +1165,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="392004040"/>
+        <c:crossAx val="2117731064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1273,6 +1273,2908 @@
           </c:marker>
           <c:val>
             <c:numRef>
+              <c:f>Sheet3!$A$1:$A$478</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="478"/>
+                <c:pt idx="0">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="277">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="279">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="280">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="281">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="285">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="286">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="287">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="288">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="289">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="290">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="291">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="292">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="293">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="294">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="295">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="296">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="297">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="298">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="299">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="300">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="301">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="302">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="303">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="304">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="305">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="306">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="307">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="308">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="309">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="310">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="311">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="312">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="313">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="314">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="315">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="316">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="317">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="318">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="319">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="320">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="321">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="322">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="323">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="324">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="325">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="326">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="327">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="328">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="329">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="330">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="331">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="332">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="333">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="334">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="335">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="336">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="337">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="338">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="339">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="340">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="341">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="342">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="343">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="344">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="345">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="346">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="347">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="348">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="349">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="350">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="351">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="352">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="353">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="354">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="355">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="356">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="357">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="358">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="359">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="360">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="361">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="362">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="363">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="364">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="365">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="366">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="367">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="368">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="369">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="370">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="371">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="372">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="373">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="374">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="375">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="376">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="377">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="378">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="379">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="380">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="381">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="382">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="383">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="384">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="385">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="386">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="387">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="388">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="389">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="390">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="391">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="392">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="393">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="394">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="395">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="396">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="397">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="398">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="399">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="400">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="401">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="402">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="403">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="404">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="405">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="406">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="407">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="408">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="409">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="410">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="411">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="412">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="413">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="414">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="415">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="416">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="417">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="418">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="419">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="420">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="421">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="422">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="423">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="424">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="425">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="426">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="427">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="428">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="429">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="430">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="431">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="432">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="433">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="434">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="435">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="436">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="437">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="438">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="439">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="440">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="441">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="442">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="443">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="444">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="445">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="446">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="447">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="448">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="449">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="450">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="451">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="452">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="453">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="454">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="455">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="456">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="457">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="458">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="459">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="460">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="461">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="462">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="463">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="464">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="465">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="466">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="467">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="468">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="469">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="470">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="471">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="472">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="473">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="474">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="475">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="476">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="477">
+                  <c:v>11.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$A$1:$A$478</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="478"/>
+                <c:pt idx="0">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="277">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="279">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="280">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="281">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="285">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="286">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="287">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="288">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="289">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="290">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="291">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="292">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="293">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="294">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="295">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="296">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="297">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="298">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="299">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="300">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="301">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="302">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="303">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="304">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="305">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="306">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="307">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="308">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="309">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="310">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="311">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="312">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="313">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="314">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="315">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="316">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="317">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="318">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="319">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="320">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="321">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="322">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="323">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="324">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="325">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="326">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="327">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="328">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="329">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="330">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="331">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="332">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="333">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="334">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="335">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="336">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="337">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="338">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="339">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="340">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="341">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="342">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="343">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="344">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="345">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="346">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="347">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="348">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="349">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="350">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="351">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="352">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="353">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="354">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="355">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="356">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="357">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="358">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="359">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="360">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="361">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="362">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="363">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="364">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="365">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="366">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="367">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="368">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="369">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="370">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="371">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="372">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="373">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="374">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="375">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="376">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="377">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="378">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="379">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="380">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="381">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="382">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="383">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="384">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="385">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="386">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="387">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="388">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="389">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="390">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="391">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="392">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="393">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="394">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="395">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="396">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="397">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="398">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="399">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="400">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="401">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="402">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="403">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="404">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="405">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="406">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="407">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="408">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="409">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="410">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="411">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="412">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="413">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="414">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="415">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="416">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="417">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="418">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="419">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="420">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="421">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="422">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="423">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="424">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="425">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="426">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="427">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="428">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="429">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="430">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="431">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="432">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="433">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="434">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="435">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="436">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="437">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="438">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="439">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="440">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="441">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="442">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="443">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="444">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="445">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="446">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="447">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="448">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="449">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="450">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="451">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="452">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="453">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="454">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="455">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="456">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="457">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="458">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="459">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="460">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="461">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="462">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="463">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="464">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="465">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="466">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="467">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="468">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="469">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="470">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="471">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="472">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="473">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="474">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="475">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="476">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="477">
+                  <c:v>11.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
               <c:f>Sheet3!$D$1:$D$478</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
@@ -2726,11 +5628,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="638959304"/>
-        <c:axId val="638971912"/>
+        <c:axId val="2123940280"/>
+        <c:axId val="2028439208"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="638959304"/>
+        <c:axId val="2123940280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2739,7 +5641,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="638971912"/>
+        <c:crossAx val="2028439208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2747,18 +5649,18 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="638971912"/>
+        <c:axId val="2028439208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="638959304"/>
+        <c:crossAx val="2123940280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4116,11 +7018,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="392082600"/>
-        <c:axId val="392085576"/>
+        <c:axId val="2117809592"/>
+        <c:axId val="2117812568"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="392082600"/>
+        <c:axId val="2117809592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4129,7 +7031,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="392085576"/>
+        <c:crossAx val="2117812568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4137,7 +7039,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="392085576"/>
+        <c:axId val="2117812568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4148,7 +7050,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="392082600"/>
+        <c:crossAx val="2117809592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6225,11 +9127,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="392126504"/>
-        <c:axId val="392129480"/>
+        <c:axId val="2117853480"/>
+        <c:axId val="2117856456"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="392126504"/>
+        <c:axId val="2117853480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6238,7 +9140,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="392129480"/>
+        <c:crossAx val="2117856456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6246,7 +9148,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="392129480"/>
+        <c:axId val="2117856456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6257,7 +9159,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="392126504"/>
+        <c:crossAx val="2117853480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7938,11 +10840,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="391466200"/>
-        <c:axId val="391463208"/>
+        <c:axId val="2117893016"/>
+        <c:axId val="2117895992"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="391466200"/>
+        <c:axId val="2117893016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7951,7 +10853,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="391463208"/>
+        <c:crossAx val="2117895992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7959,7 +10861,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="391463208"/>
+        <c:axId val="2117895992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7970,7 +10872,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="391466200"/>
+        <c:crossAx val="2117893016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11655,11 +14557,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="391426968"/>
-        <c:axId val="391423976"/>
+        <c:axId val="2117932296"/>
+        <c:axId val="2117935272"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="391426968"/>
+        <c:axId val="2117932296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11668,7 +14570,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="391423976"/>
+        <c:crossAx val="2117935272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11676,7 +14578,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="391423976"/>
+        <c:axId val="2117935272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11687,7 +14589,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="391426968"/>
+        <c:crossAx val="2117932296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12754,11 +15656,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="391385624"/>
-        <c:axId val="391375832"/>
+        <c:axId val="2117976968"/>
+        <c:axId val="2117979912"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="391385624"/>
+        <c:axId val="2117976968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12767,7 +15669,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="391375832"/>
+        <c:crossAx val="2117979912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12775,7 +15677,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="391375832"/>
+        <c:axId val="2117979912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12786,7 +15688,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="391385624"/>
+        <c:crossAx val="2117976968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15349,11 +18251,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="391338504"/>
-        <c:axId val="391335512"/>
+        <c:axId val="2118017256"/>
+        <c:axId val="2118020232"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="391338504"/>
+        <c:axId val="2118017256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15362,7 +18264,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="391335512"/>
+        <c:crossAx val="2118020232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15370,7 +18272,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="391335512"/>
+        <c:axId val="2118020232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15381,7 +18283,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="391338504"/>
+        <c:crossAx val="2118017256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -19594,11 +22496,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="391298040"/>
-        <c:axId val="391295048"/>
+        <c:axId val="2118058232"/>
+        <c:axId val="2118061208"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="391298040"/>
+        <c:axId val="2118058232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19607,7 +22509,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="391295048"/>
+        <c:crossAx val="2118061208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -19615,7 +22517,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="391295048"/>
+        <c:axId val="2118061208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19626,7 +22528,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="391298040"/>
+        <c:crossAx val="2118058232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -20821,11 +23723,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="391254664"/>
-        <c:axId val="391251672"/>
+        <c:axId val="2118101096"/>
+        <c:axId val="2118104072"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="391254664"/>
+        <c:axId val="2118101096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20834,7 +23736,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="391251672"/>
+        <c:crossAx val="2118104072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -20842,7 +23744,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="391251672"/>
+        <c:axId val="2118104072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20853,14 +23755,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="391254664"/>
+        <c:crossAx val="2118101096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -21471,19 +24372,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
+      <xdr:colOff>165100</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>127000</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -26543,7 +29444,7 @@
   <dimension ref="A1:D478"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -46501,7 +49402,7 @@
         <v>15</v>
       </c>
       <c r="E98">
-        <f t="shared" ref="E98:E129" si="5">D98/$L$2</f>
+        <f t="shared" ref="E98:E121" si="5">D98/$L$2</f>
         <v>0.5</v>
       </c>
     </row>

</xml_diff>